<commit_message>
plan van aanpak checklist
</commit_message>
<xml_diff>
--- a/Documentatie/1.5 Plan van aanpak/plan van aanpak checklist.xlsx
+++ b/Documentatie/1.5 Plan van aanpak/plan van aanpak checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Teun\School\MED Leerjaar 3 Periode_11\Project\Documentatie\1.5 Plan van aanpak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorri\Documents\Rooster-App\Documentatie\1.5 Plan van aanpak\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">A Algemeen, lay-out en taalgebruik van het plan van aanpak </t>
   </si>
@@ -300,12 +300,15 @@
   </si>
   <si>
     <t>Checklist Plan van Aanpak</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -629,6 +632,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -664,6 +684,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -840,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C114"/>
+  <dimension ref="A2:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1094,9 @@
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
       <c r="C28">
         <v>1</v>
       </c>
@@ -1066,7 +1105,9 @@
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="13">
+        <v>1</v>
+      </c>
       <c r="C29">
         <v>1</v>
       </c>
@@ -1371,7 +1412,9 @@
       <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="13"/>
+      <c r="B65" s="13">
+        <v>1</v>
+      </c>
       <c r="C65">
         <v>1</v>
       </c>
@@ -1380,7 +1423,9 @@
       <c r="A66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="13"/>
+      <c r="B66" s="13">
+        <v>1</v>
+      </c>
       <c r="C66">
         <v>1</v>
       </c>
@@ -1389,7 +1434,9 @@
       <c r="A67" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="13"/>
+      <c r="B67" s="13">
+        <v>1</v>
+      </c>
       <c r="C67">
         <v>1</v>
       </c>
@@ -1398,7 +1445,9 @@
       <c r="A68" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="13"/>
+      <c r="B68" s="13">
+        <v>1</v>
+      </c>
       <c r="C68">
         <v>1</v>
       </c>
@@ -1417,7 +1466,9 @@
       <c r="A71" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B71" s="13"/>
+      <c r="B71" s="13">
+        <v>1</v>
+      </c>
       <c r="C71">
         <v>1</v>
       </c>
@@ -1426,7 +1477,9 @@
       <c r="A72" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="13">
+        <v>1</v>
+      </c>
       <c r="C72">
         <v>1</v>
       </c>
@@ -1435,7 +1488,9 @@
       <c r="A73" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="13"/>
+      <c r="B73" s="13">
+        <v>1</v>
+      </c>
       <c r="C73">
         <v>1</v>
       </c>
@@ -1453,7 +1508,9 @@
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="13"/>
+      <c r="B75" s="13">
+        <v>1</v>
+      </c>
       <c r="C75">
         <v>1</v>
       </c>
@@ -1462,7 +1519,9 @@
       <c r="A76" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="13"/>
+      <c r="B76" s="13">
+        <v>1</v>
+      </c>
       <c r="C76">
         <v>1</v>
       </c>
@@ -1480,7 +1539,9 @@
       <c r="A78" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="13">
+        <v>1</v>
+      </c>
       <c r="C78">
         <v>1</v>
       </c>
@@ -1495,108 +1556,126 @@
       </c>
       <c r="B80" s="12"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="12"/>
     </row>
-    <row r="82" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B82" s="12"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="13"/>
+      <c r="B83" s="13">
+        <v>1</v>
+      </c>
       <c r="C83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B84" s="13"/>
+      <c r="B84" s="13">
+        <v>1</v>
+      </c>
       <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="13"/>
+      <c r="B85" s="13">
+        <v>1</v>
+      </c>
       <c r="C85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B86" s="13"/>
+      <c r="B86" s="13">
+        <v>1</v>
+      </c>
       <c r="C86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="12"/>
     </row>
-    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B88" s="12"/>
     </row>
-    <row r="89" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="13"/>
+      <c r="B89" s="13">
+        <v>1</v>
+      </c>
       <c r="C89">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B90" s="13"/>
+      <c r="B90" s="13">
+        <v>1</v>
+      </c>
       <c r="C90">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B91" s="13"/>
+      <c r="B91" s="13">
+        <v>1</v>
+      </c>
       <c r="C91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B92" s="13"/>
+      <c r="B92" s="13">
+        <v>1</v>
+      </c>
       <c r="C92">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="13"/>
+      <c r="B93" s="13">
+        <v>1</v>
+      </c>
       <c r="C93">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>74</v>
       </c>
@@ -1605,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>75</v>
       </c>
@@ -1614,9 +1693,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="12"/>
+      <c r="D96" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
@@ -1628,7 +1710,9 @@
       <c r="A98" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B98" s="13"/>
+      <c r="B98" s="13">
+        <v>1</v>
+      </c>
       <c r="C98">
         <v>1</v>
       </c>
@@ -1637,7 +1721,9 @@
       <c r="A99" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B99" s="13"/>
+      <c r="B99" s="13">
+        <v>1</v>
+      </c>
       <c r="C99">
         <v>1</v>
       </c>
@@ -1646,7 +1732,9 @@
       <c r="A100" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="13"/>
+      <c r="B100" s="13">
+        <v>1</v>
+      </c>
       <c r="C100">
         <v>1</v>
       </c>
@@ -1665,7 +1753,9 @@
       <c r="A103" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B103" s="13"/>
+      <c r="B103" s="13">
+        <v>1</v>
+      </c>
       <c r="C103">
         <v>1</v>
       </c>
@@ -1674,7 +1764,9 @@
       <c r="A104" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B104" s="13"/>
+      <c r="B104" s="13">
+        <v>1</v>
+      </c>
       <c r="C104">
         <v>1</v>
       </c>
@@ -1692,7 +1784,9 @@
       <c r="A106" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B106" s="13"/>
+      <c r="B106" s="13">
+        <v>1</v>
+      </c>
       <c r="C106">
         <v>1</v>
       </c>
@@ -1701,7 +1795,9 @@
       <c r="A107" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B107" s="13"/>
+      <c r="B107" s="13">
+        <v>1</v>
+      </c>
       <c r="C107">
         <v>1</v>
       </c>
@@ -1720,7 +1816,9 @@
       <c r="A110" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B110" s="16"/>
+      <c r="B110" s="16">
+        <v>1</v>
+      </c>
       <c r="C110">
         <v>1</v>
       </c>
@@ -1731,7 +1829,7 @@
       </c>
       <c r="B111">
         <f t="shared" ref="B111:C111" si="0">SUM(B8:B110)</f>
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C111">
         <f t="shared" si="0"/>
@@ -1744,7 +1842,7 @@
       </c>
       <c r="B112" s="10">
         <f>B111/$C111*10</f>
-        <v>4.1428571428571432</v>
+        <v>8.2857142857142865</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
@@ -1796,18 +1894,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1860,6 +1958,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F9E84F0-AD95-425C-8EB4-A1D207D50D88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4D51CB1-8E52-45C8-99E7-CF80D4D7E80D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1869,14 +1975,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F9E84F0-AD95-425C-8EB4-A1D207D50D88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>